<commit_message>
Alteração do Loop Infinito Ar Condicionado
</commit_message>
<xml_diff>
--- a/tempo.xlsx
+++ b/tempo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Projeto_Final_GIT_GITHUB\Start-Stop-System---Projeto-Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11736"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16176" windowHeight="5112"/>
   </bookViews>
   <sheets>
     <sheet name="tempo" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,12 +361,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -533,8 +527,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -896,15 +890,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1512"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1461" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F1516" sqref="F1516"/>
+    <sheetView tabSelected="1" topLeftCell="A1496" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L1505" sqref="L1505"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Planilha Nova & Lógica EPB ajustada
</commit_message>
<xml_diff>
--- a/tempo.xlsx
+++ b/tempo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65e57b1b17248dcf/Residencia_Tecnologica_Stellantis_UFPE/Projeto Final/Start-Stop-System---Projeto-Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79C2CDF6-D000-48B7-9DA0-7600F62DEF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0AF7280-2301-4655-B1B6-4E32870E071F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1860"/>
+  <dimension ref="A1:D2092"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="A2069" workbookViewId="0">
+      <selection activeCell="F2093" sqref="F2093"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26447,6 +26447,3254 @@
         <v>0</v>
       </c>
     </row>
+    <row r="1861" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1861">
+        <v>186.9</v>
+      </c>
+      <c r="B1861">
+        <v>0</v>
+      </c>
+      <c r="C1861">
+        <v>0.05</v>
+      </c>
+      <c r="D1861">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1862" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1862">
+        <v>187</v>
+      </c>
+      <c r="B1862">
+        <v>0</v>
+      </c>
+      <c r="C1862">
+        <v>0.04</v>
+      </c>
+      <c r="D1862">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1863" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1863">
+        <v>187.1</v>
+      </c>
+      <c r="B1863">
+        <v>0</v>
+      </c>
+      <c r="C1863">
+        <v>0.03</v>
+      </c>
+      <c r="D1863">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1864" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1864">
+        <v>187.2</v>
+      </c>
+      <c r="B1864">
+        <v>0</v>
+      </c>
+      <c r="C1864">
+        <v>0.01</v>
+      </c>
+      <c r="D1864">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1865" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1865">
+        <v>187.3</v>
+      </c>
+      <c r="B1865">
+        <v>0</v>
+      </c>
+      <c r="C1865">
+        <v>0</v>
+      </c>
+      <c r="D1865">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1866" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1866">
+        <v>187.4</v>
+      </c>
+      <c r="B1866">
+        <v>0</v>
+      </c>
+      <c r="C1866">
+        <v>0</v>
+      </c>
+      <c r="D1866">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1867">
+        <v>187.5</v>
+      </c>
+      <c r="B1867">
+        <v>0</v>
+      </c>
+      <c r="C1867">
+        <v>0</v>
+      </c>
+      <c r="D1867">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1868">
+        <v>187.6</v>
+      </c>
+      <c r="B1868">
+        <v>0</v>
+      </c>
+      <c r="C1868">
+        <v>0</v>
+      </c>
+      <c r="D1868">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1869" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1869">
+        <v>187.7</v>
+      </c>
+      <c r="B1869">
+        <v>0</v>
+      </c>
+      <c r="C1869">
+        <v>0</v>
+      </c>
+      <c r="D1869">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1870" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1870">
+        <v>187.8</v>
+      </c>
+      <c r="B1870">
+        <v>0</v>
+      </c>
+      <c r="C1870">
+        <v>0</v>
+      </c>
+      <c r="D1870">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1871" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1871">
+        <v>187.9</v>
+      </c>
+      <c r="B1871">
+        <v>0</v>
+      </c>
+      <c r="C1871">
+        <v>0</v>
+      </c>
+      <c r="D1871">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1872">
+        <v>188</v>
+      </c>
+      <c r="B1872">
+        <v>0</v>
+      </c>
+      <c r="C1872">
+        <v>0</v>
+      </c>
+      <c r="D1872">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1873" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1873">
+        <v>188.1</v>
+      </c>
+      <c r="B1873">
+        <v>0</v>
+      </c>
+      <c r="C1873">
+        <v>0</v>
+      </c>
+      <c r="D1873">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1874">
+        <v>188.2</v>
+      </c>
+      <c r="B1874">
+        <v>0</v>
+      </c>
+      <c r="C1874">
+        <v>0</v>
+      </c>
+      <c r="D1874">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1875" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1875">
+        <v>188.3</v>
+      </c>
+      <c r="B1875">
+        <v>0</v>
+      </c>
+      <c r="C1875">
+        <v>0</v>
+      </c>
+      <c r="D1875">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1876">
+        <v>188.4</v>
+      </c>
+      <c r="B1876">
+        <v>0</v>
+      </c>
+      <c r="C1876">
+        <v>0</v>
+      </c>
+      <c r="D1876">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1877" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1877">
+        <v>188.5</v>
+      </c>
+      <c r="B1877">
+        <v>0</v>
+      </c>
+      <c r="C1877">
+        <v>0</v>
+      </c>
+      <c r="D1877">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1878" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1878">
+        <v>188.6</v>
+      </c>
+      <c r="B1878">
+        <v>0</v>
+      </c>
+      <c r="C1878">
+        <v>0</v>
+      </c>
+      <c r="D1878">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1879" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1879">
+        <v>188.7</v>
+      </c>
+      <c r="B1879">
+        <v>0</v>
+      </c>
+      <c r="C1879">
+        <v>0</v>
+      </c>
+      <c r="D1879">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1880">
+        <v>188.8</v>
+      </c>
+      <c r="B1880">
+        <v>0</v>
+      </c>
+      <c r="C1880">
+        <v>0</v>
+      </c>
+      <c r="D1880">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1881">
+        <v>188.9</v>
+      </c>
+      <c r="B1881">
+        <v>0</v>
+      </c>
+      <c r="C1881">
+        <v>0</v>
+      </c>
+      <c r="D1881">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1882" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1882">
+        <v>189</v>
+      </c>
+      <c r="B1882">
+        <v>0</v>
+      </c>
+      <c r="C1882">
+        <v>0</v>
+      </c>
+      <c r="D1882">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1883" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1883">
+        <v>189.1</v>
+      </c>
+      <c r="B1883">
+        <v>0</v>
+      </c>
+      <c r="C1883">
+        <v>0</v>
+      </c>
+      <c r="D1883">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1884">
+        <v>189.2</v>
+      </c>
+      <c r="B1884">
+        <v>0</v>
+      </c>
+      <c r="C1884">
+        <v>0</v>
+      </c>
+      <c r="D1884">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1885" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1885">
+        <v>189.3</v>
+      </c>
+      <c r="B1885">
+        <v>0</v>
+      </c>
+      <c r="C1885">
+        <v>0</v>
+      </c>
+      <c r="D1885">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1886" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1886">
+        <v>189.4</v>
+      </c>
+      <c r="B1886">
+        <v>0</v>
+      </c>
+      <c r="C1886">
+        <v>0</v>
+      </c>
+      <c r="D1886">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1887" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1887">
+        <v>189.5</v>
+      </c>
+      <c r="B1887">
+        <v>0</v>
+      </c>
+      <c r="C1887">
+        <v>0</v>
+      </c>
+      <c r="D1887">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1888" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1888">
+        <v>189.6</v>
+      </c>
+      <c r="B1888">
+        <v>0</v>
+      </c>
+      <c r="C1888">
+        <v>0</v>
+      </c>
+      <c r="D1888">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1889" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1889">
+        <v>189.7</v>
+      </c>
+      <c r="B1889">
+        <v>0</v>
+      </c>
+      <c r="C1889">
+        <v>0</v>
+      </c>
+      <c r="D1889">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1890" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1890">
+        <v>189.8</v>
+      </c>
+      <c r="B1890">
+        <v>0</v>
+      </c>
+      <c r="C1890">
+        <v>0</v>
+      </c>
+      <c r="D1890">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1891" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1891">
+        <v>189.9</v>
+      </c>
+      <c r="B1891">
+        <v>0</v>
+      </c>
+      <c r="C1891">
+        <v>0</v>
+      </c>
+      <c r="D1891">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1892" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1892">
+        <v>190</v>
+      </c>
+      <c r="B1892">
+        <v>0</v>
+      </c>
+      <c r="C1892">
+        <v>0</v>
+      </c>
+      <c r="D1892">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1893" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1893">
+        <v>190.1</v>
+      </c>
+      <c r="B1893">
+        <v>0</v>
+      </c>
+      <c r="C1893">
+        <v>0</v>
+      </c>
+      <c r="D1893">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1894" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1894">
+        <v>190.2</v>
+      </c>
+      <c r="B1894">
+        <v>0</v>
+      </c>
+      <c r="C1894">
+        <v>0</v>
+      </c>
+      <c r="D1894">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1895" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1895">
+        <v>190.3</v>
+      </c>
+      <c r="B1895">
+        <v>0</v>
+      </c>
+      <c r="C1895">
+        <v>0</v>
+      </c>
+      <c r="D1895">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1896" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1896">
+        <v>190.4</v>
+      </c>
+      <c r="B1896">
+        <v>0</v>
+      </c>
+      <c r="C1896">
+        <v>0</v>
+      </c>
+      <c r="D1896">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1897" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1897">
+        <v>190.5</v>
+      </c>
+      <c r="B1897">
+        <v>0</v>
+      </c>
+      <c r="C1897">
+        <v>0</v>
+      </c>
+      <c r="D1897">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1898" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1898">
+        <v>190.6</v>
+      </c>
+      <c r="B1898">
+        <v>0</v>
+      </c>
+      <c r="C1898">
+        <v>0</v>
+      </c>
+      <c r="D1898">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1899" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1899">
+        <v>190.7</v>
+      </c>
+      <c r="B1899">
+        <v>0</v>
+      </c>
+      <c r="C1899">
+        <v>0</v>
+      </c>
+      <c r="D1899">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1900" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1900">
+        <v>190.8</v>
+      </c>
+      <c r="B1900">
+        <v>0</v>
+      </c>
+      <c r="C1900">
+        <v>0</v>
+      </c>
+      <c r="D1900">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1901" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1901">
+        <v>190.9</v>
+      </c>
+      <c r="B1901">
+        <v>0</v>
+      </c>
+      <c r="C1901">
+        <v>0</v>
+      </c>
+      <c r="D1901">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1902" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1902">
+        <v>191</v>
+      </c>
+      <c r="B1902">
+        <v>0</v>
+      </c>
+      <c r="C1902">
+        <v>0</v>
+      </c>
+      <c r="D1902">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1903" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1903">
+        <v>191.1</v>
+      </c>
+      <c r="B1903">
+        <v>0</v>
+      </c>
+      <c r="C1903">
+        <v>0</v>
+      </c>
+      <c r="D1903">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1904" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1904">
+        <v>191.2</v>
+      </c>
+      <c r="B1904">
+        <v>0</v>
+      </c>
+      <c r="C1904">
+        <v>0</v>
+      </c>
+      <c r="D1904">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1905" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1905">
+        <v>191.3</v>
+      </c>
+      <c r="B1905">
+        <v>0</v>
+      </c>
+      <c r="C1905">
+        <v>0</v>
+      </c>
+      <c r="D1905">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1906" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1906">
+        <v>191.4</v>
+      </c>
+      <c r="B1906">
+        <v>0</v>
+      </c>
+      <c r="C1906">
+        <v>0</v>
+      </c>
+      <c r="D1906">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1907" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1907">
+        <v>191.5</v>
+      </c>
+      <c r="B1907">
+        <v>0</v>
+      </c>
+      <c r="C1907">
+        <v>0</v>
+      </c>
+      <c r="D1907">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1908" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1908">
+        <v>191.6</v>
+      </c>
+      <c r="B1908">
+        <v>0</v>
+      </c>
+      <c r="C1908">
+        <v>0</v>
+      </c>
+      <c r="D1908">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1909" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1909">
+        <v>191.7</v>
+      </c>
+      <c r="B1909">
+        <v>0</v>
+      </c>
+      <c r="C1909">
+        <v>0</v>
+      </c>
+      <c r="D1909">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1910" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1910">
+        <v>191.8</v>
+      </c>
+      <c r="B1910">
+        <v>0</v>
+      </c>
+      <c r="C1910">
+        <v>0</v>
+      </c>
+      <c r="D1910">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1911" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1911">
+        <v>191.9</v>
+      </c>
+      <c r="B1911">
+        <v>0</v>
+      </c>
+      <c r="C1911">
+        <v>0</v>
+      </c>
+      <c r="D1911">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1912" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1912">
+        <v>192</v>
+      </c>
+      <c r="B1912">
+        <v>0</v>
+      </c>
+      <c r="C1912">
+        <v>0</v>
+      </c>
+      <c r="D1912">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1913" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1913">
+        <v>192.1</v>
+      </c>
+      <c r="B1913">
+        <v>0</v>
+      </c>
+      <c r="C1913">
+        <v>0</v>
+      </c>
+      <c r="D1913">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1914" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1914">
+        <v>192.2</v>
+      </c>
+      <c r="B1914">
+        <v>0</v>
+      </c>
+      <c r="C1914">
+        <v>0</v>
+      </c>
+      <c r="D1914">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1915" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1915">
+        <v>192.3</v>
+      </c>
+      <c r="B1915">
+        <v>0</v>
+      </c>
+      <c r="C1915">
+        <v>0</v>
+      </c>
+      <c r="D1915">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1916" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1916">
+        <v>192.4</v>
+      </c>
+      <c r="B1916">
+        <v>0</v>
+      </c>
+      <c r="C1916">
+        <v>0</v>
+      </c>
+      <c r="D1916">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1917" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1917">
+        <v>192.5</v>
+      </c>
+      <c r="B1917">
+        <v>0</v>
+      </c>
+      <c r="C1917">
+        <v>0</v>
+      </c>
+      <c r="D1917">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1918" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1918">
+        <v>192.6</v>
+      </c>
+      <c r="B1918">
+        <v>0</v>
+      </c>
+      <c r="C1918">
+        <v>0</v>
+      </c>
+      <c r="D1918">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1919" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1919">
+        <v>192.7</v>
+      </c>
+      <c r="B1919">
+        <v>0</v>
+      </c>
+      <c r="C1919">
+        <v>0</v>
+      </c>
+      <c r="D1919">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1920" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1920">
+        <v>192.8</v>
+      </c>
+      <c r="B1920">
+        <v>0</v>
+      </c>
+      <c r="C1920">
+        <v>0</v>
+      </c>
+      <c r="D1920">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1921" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1921">
+        <v>192.9</v>
+      </c>
+      <c r="B1921">
+        <v>0</v>
+      </c>
+      <c r="C1921">
+        <v>0</v>
+      </c>
+      <c r="D1921">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1922" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1922">
+        <v>193</v>
+      </c>
+      <c r="B1922">
+        <v>0</v>
+      </c>
+      <c r="C1922">
+        <v>0</v>
+      </c>
+      <c r="D1922">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1923" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1923">
+        <v>193.1</v>
+      </c>
+      <c r="B1923">
+        <v>0</v>
+      </c>
+      <c r="C1923">
+        <v>0</v>
+      </c>
+      <c r="D1923">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1924" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1924">
+        <v>193.2</v>
+      </c>
+      <c r="B1924">
+        <v>0</v>
+      </c>
+      <c r="C1924">
+        <v>0</v>
+      </c>
+      <c r="D1924">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1925" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1925">
+        <v>193.3</v>
+      </c>
+      <c r="B1925">
+        <v>0</v>
+      </c>
+      <c r="C1925">
+        <v>0</v>
+      </c>
+      <c r="D1925">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1926" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1926">
+        <v>193.4</v>
+      </c>
+      <c r="B1926">
+        <v>0</v>
+      </c>
+      <c r="C1926">
+        <v>0</v>
+      </c>
+      <c r="D1926">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1927" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1927">
+        <v>193.5</v>
+      </c>
+      <c r="B1927">
+        <v>0</v>
+      </c>
+      <c r="C1927">
+        <v>0</v>
+      </c>
+      <c r="D1927">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1928" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1928">
+        <v>193.6</v>
+      </c>
+      <c r="B1928">
+        <v>0</v>
+      </c>
+      <c r="C1928">
+        <v>0</v>
+      </c>
+      <c r="D1928">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1929" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1929">
+        <v>193.7</v>
+      </c>
+      <c r="B1929">
+        <v>0</v>
+      </c>
+      <c r="C1929">
+        <v>0</v>
+      </c>
+      <c r="D1929">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1930" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1930">
+        <v>193.8</v>
+      </c>
+      <c r="B1930">
+        <v>0</v>
+      </c>
+      <c r="C1930">
+        <v>0</v>
+      </c>
+      <c r="D1930">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1931" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1931">
+        <v>193.9</v>
+      </c>
+      <c r="B1931">
+        <v>0</v>
+      </c>
+      <c r="C1931">
+        <v>0</v>
+      </c>
+      <c r="D1931">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1932" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1932">
+        <v>194</v>
+      </c>
+      <c r="B1932">
+        <v>0</v>
+      </c>
+      <c r="C1932">
+        <v>0</v>
+      </c>
+      <c r="D1932">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1933" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1933">
+        <v>194.1</v>
+      </c>
+      <c r="B1933">
+        <v>0</v>
+      </c>
+      <c r="C1933">
+        <v>0</v>
+      </c>
+      <c r="D1933">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1934" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1934">
+        <v>194.2</v>
+      </c>
+      <c r="B1934">
+        <v>0</v>
+      </c>
+      <c r="C1934">
+        <v>0</v>
+      </c>
+      <c r="D1934">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1935" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1935">
+        <v>194.3</v>
+      </c>
+      <c r="B1935">
+        <v>0</v>
+      </c>
+      <c r="C1935">
+        <v>0</v>
+      </c>
+      <c r="D1935">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1936" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1936">
+        <v>194.4</v>
+      </c>
+      <c r="B1936">
+        <v>0</v>
+      </c>
+      <c r="C1936">
+        <v>0</v>
+      </c>
+      <c r="D1936">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1937" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1937">
+        <v>194.5</v>
+      </c>
+      <c r="B1937">
+        <v>0</v>
+      </c>
+      <c r="C1937">
+        <v>0</v>
+      </c>
+      <c r="D1937">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1938" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1938">
+        <v>194.6</v>
+      </c>
+      <c r="B1938">
+        <v>0</v>
+      </c>
+      <c r="C1938">
+        <v>0</v>
+      </c>
+      <c r="D1938">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1939" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1939">
+        <v>194.7</v>
+      </c>
+      <c r="B1939">
+        <v>0</v>
+      </c>
+      <c r="C1939">
+        <v>0</v>
+      </c>
+      <c r="D1939">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1940" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1940">
+        <v>194.8</v>
+      </c>
+      <c r="B1940">
+        <v>0</v>
+      </c>
+      <c r="C1940">
+        <v>0</v>
+      </c>
+      <c r="D1940">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1941" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1941">
+        <v>194.9</v>
+      </c>
+      <c r="B1941">
+        <v>0</v>
+      </c>
+      <c r="C1941">
+        <v>0</v>
+      </c>
+      <c r="D1941">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1942" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1942">
+        <v>195</v>
+      </c>
+      <c r="B1942">
+        <v>0</v>
+      </c>
+      <c r="C1942">
+        <v>0</v>
+      </c>
+      <c r="D1942">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1943" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1943">
+        <v>195.1</v>
+      </c>
+      <c r="B1943">
+        <v>0</v>
+      </c>
+      <c r="C1943">
+        <v>0</v>
+      </c>
+      <c r="D1943">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1944" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1944">
+        <v>195.2</v>
+      </c>
+      <c r="B1944">
+        <v>0</v>
+      </c>
+      <c r="C1944">
+        <v>0</v>
+      </c>
+      <c r="D1944">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1945" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1945">
+        <v>195.29999999999899</v>
+      </c>
+      <c r="B1945">
+        <v>0</v>
+      </c>
+      <c r="C1945">
+        <v>0</v>
+      </c>
+      <c r="D1945">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1946" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1946">
+        <v>195.39999999999901</v>
+      </c>
+      <c r="B1946">
+        <v>0</v>
+      </c>
+      <c r="C1946">
+        <v>0</v>
+      </c>
+      <c r="D1946">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1947">
+        <v>195.49999999999901</v>
+      </c>
+      <c r="B1947">
+        <v>0</v>
+      </c>
+      <c r="C1947">
+        <v>0</v>
+      </c>
+      <c r="D1947">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1948" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1948">
+        <v>195.599999999999</v>
+      </c>
+      <c r="B1948">
+        <v>0</v>
+      </c>
+      <c r="C1948">
+        <v>0</v>
+      </c>
+      <c r="D1948">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1949" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1949">
+        <v>195.69999999999899</v>
+      </c>
+      <c r="B1949">
+        <v>0</v>
+      </c>
+      <c r="C1949">
+        <v>0</v>
+      </c>
+      <c r="D1949">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1950" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1950">
+        <v>195.79999999999899</v>
+      </c>
+      <c r="B1950">
+        <v>0</v>
+      </c>
+      <c r="C1950">
+        <v>0</v>
+      </c>
+      <c r="D1950">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1951" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1951">
+        <v>195.89999999999901</v>
+      </c>
+      <c r="B1951">
+        <v>0</v>
+      </c>
+      <c r="C1951">
+        <v>0</v>
+      </c>
+      <c r="D1951">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1952" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1952">
+        <v>195.99999999999901</v>
+      </c>
+      <c r="B1952">
+        <v>0</v>
+      </c>
+      <c r="C1952">
+        <v>0</v>
+      </c>
+      <c r="D1952">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1953" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1953">
+        <v>196.099999999999</v>
+      </c>
+      <c r="B1953">
+        <v>0</v>
+      </c>
+      <c r="C1953">
+        <v>0</v>
+      </c>
+      <c r="D1953">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1954" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1954">
+        <v>196.19999999999899</v>
+      </c>
+      <c r="B1954">
+        <v>0</v>
+      </c>
+      <c r="C1954">
+        <v>0</v>
+      </c>
+      <c r="D1954">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1955" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1955">
+        <v>196.29999999999899</v>
+      </c>
+      <c r="B1955">
+        <v>0</v>
+      </c>
+      <c r="C1955">
+        <v>0</v>
+      </c>
+      <c r="D1955">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1956" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1956">
+        <v>196.39999999999901</v>
+      </c>
+      <c r="B1956">
+        <v>0</v>
+      </c>
+      <c r="C1956">
+        <v>0</v>
+      </c>
+      <c r="D1956">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1957" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1957">
+        <v>196.49999999999901</v>
+      </c>
+      <c r="B1957">
+        <v>0</v>
+      </c>
+      <c r="C1957">
+        <v>0</v>
+      </c>
+      <c r="D1957">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1958" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1958">
+        <v>196.599999999999</v>
+      </c>
+      <c r="B1958">
+        <v>0</v>
+      </c>
+      <c r="C1958">
+        <v>0</v>
+      </c>
+      <c r="D1958">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1959" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1959">
+        <v>196.69999999999899</v>
+      </c>
+      <c r="B1959">
+        <v>0</v>
+      </c>
+      <c r="C1959">
+        <v>0</v>
+      </c>
+      <c r="D1959">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1960" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1960">
+        <v>196.79999999999899</v>
+      </c>
+      <c r="B1960">
+        <v>0</v>
+      </c>
+      <c r="C1960">
+        <v>0</v>
+      </c>
+      <c r="D1960">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1961" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1961">
+        <v>196.89999999999901</v>
+      </c>
+      <c r="B1961">
+        <v>0</v>
+      </c>
+      <c r="C1961">
+        <v>0</v>
+      </c>
+      <c r="D1961">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1962" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1962">
+        <v>196.99999999999901</v>
+      </c>
+      <c r="B1962">
+        <v>0</v>
+      </c>
+      <c r="C1962">
+        <v>0</v>
+      </c>
+      <c r="D1962">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1963" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1963">
+        <v>197.099999999999</v>
+      </c>
+      <c r="B1963">
+        <v>0</v>
+      </c>
+      <c r="C1963">
+        <v>0</v>
+      </c>
+      <c r="D1963">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1964" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1964">
+        <v>197.19999999999899</v>
+      </c>
+      <c r="B1964">
+        <v>0</v>
+      </c>
+      <c r="C1964">
+        <v>0</v>
+      </c>
+      <c r="D1964">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1965" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1965">
+        <v>197.29999999999899</v>
+      </c>
+      <c r="B1965">
+        <v>0</v>
+      </c>
+      <c r="C1965">
+        <v>0</v>
+      </c>
+      <c r="D1965">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1966" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1966">
+        <v>197.39999999999901</v>
+      </c>
+      <c r="B1966">
+        <v>0</v>
+      </c>
+      <c r="C1966">
+        <v>0</v>
+      </c>
+      <c r="D1966">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1967" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1967">
+        <v>197.49999999999901</v>
+      </c>
+      <c r="B1967">
+        <v>0</v>
+      </c>
+      <c r="C1967">
+        <v>0</v>
+      </c>
+      <c r="D1967">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1968" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1968">
+        <v>197.599999999999</v>
+      </c>
+      <c r="B1968">
+        <v>0</v>
+      </c>
+      <c r="C1968">
+        <v>0</v>
+      </c>
+      <c r="D1968">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1969" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1969">
+        <v>197.69999999999899</v>
+      </c>
+      <c r="B1969">
+        <v>0</v>
+      </c>
+      <c r="C1969">
+        <v>0</v>
+      </c>
+      <c r="D1969">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1970" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1970">
+        <v>197.79999999999899</v>
+      </c>
+      <c r="B1970">
+        <v>0</v>
+      </c>
+      <c r="C1970">
+        <v>0</v>
+      </c>
+      <c r="D1970">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1971" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1971">
+        <v>197.89999999999901</v>
+      </c>
+      <c r="B1971">
+        <v>0</v>
+      </c>
+      <c r="C1971">
+        <v>0</v>
+      </c>
+      <c r="D1971">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1972" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1972">
+        <v>197.99999999999901</v>
+      </c>
+      <c r="B1972">
+        <v>0</v>
+      </c>
+      <c r="C1972">
+        <v>0</v>
+      </c>
+      <c r="D1972">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1973" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1973">
+        <v>198.099999999999</v>
+      </c>
+      <c r="B1973">
+        <v>0</v>
+      </c>
+      <c r="C1973">
+        <v>0</v>
+      </c>
+      <c r="D1973">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1974" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1974">
+        <v>198.19999999999899</v>
+      </c>
+      <c r="B1974">
+        <v>0</v>
+      </c>
+      <c r="C1974">
+        <v>0</v>
+      </c>
+      <c r="D1974">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1975" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1975">
+        <v>198.29999999999899</v>
+      </c>
+      <c r="B1975">
+        <v>0</v>
+      </c>
+      <c r="C1975">
+        <v>0</v>
+      </c>
+      <c r="D1975">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1976" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1976">
+        <v>198.39999999999901</v>
+      </c>
+      <c r="B1976">
+        <v>0</v>
+      </c>
+      <c r="C1976">
+        <v>0</v>
+      </c>
+      <c r="D1976">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1977" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1977">
+        <v>198.49999999999901</v>
+      </c>
+      <c r="B1977">
+        <v>0</v>
+      </c>
+      <c r="C1977">
+        <v>0</v>
+      </c>
+      <c r="D1977">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1978" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1978">
+        <v>198.599999999999</v>
+      </c>
+      <c r="B1978">
+        <v>0</v>
+      </c>
+      <c r="C1978">
+        <v>0</v>
+      </c>
+      <c r="D1978">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1979" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1979">
+        <v>198.69999999999899</v>
+      </c>
+      <c r="B1979">
+        <v>0</v>
+      </c>
+      <c r="C1979">
+        <v>0</v>
+      </c>
+      <c r="D1979">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1980" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1980">
+        <v>198.79999999999899</v>
+      </c>
+      <c r="B1980">
+        <v>0</v>
+      </c>
+      <c r="C1980">
+        <v>0</v>
+      </c>
+      <c r="D1980">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1981" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1981">
+        <v>198.89999999999901</v>
+      </c>
+      <c r="B1981">
+        <v>0</v>
+      </c>
+      <c r="C1981">
+        <v>0</v>
+      </c>
+      <c r="D1981">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1982" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1982">
+        <v>198.99999999999901</v>
+      </c>
+      <c r="B1982">
+        <v>0</v>
+      </c>
+      <c r="C1982">
+        <v>0</v>
+      </c>
+      <c r="D1982">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1983" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1983">
+        <v>199.099999999999</v>
+      </c>
+      <c r="B1983">
+        <v>0</v>
+      </c>
+      <c r="C1983">
+        <v>0</v>
+      </c>
+      <c r="D1983">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1984" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1984">
+        <v>199.19999999999899</v>
+      </c>
+      <c r="B1984">
+        <v>0</v>
+      </c>
+      <c r="C1984">
+        <v>0</v>
+      </c>
+      <c r="D1984">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1985" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1985">
+        <v>199.29999999999899</v>
+      </c>
+      <c r="B1985">
+        <v>0</v>
+      </c>
+      <c r="C1985">
+        <v>0</v>
+      </c>
+      <c r="D1985">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1986" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1986">
+        <v>199.39999999999901</v>
+      </c>
+      <c r="B1986">
+        <v>0</v>
+      </c>
+      <c r="C1986">
+        <v>0</v>
+      </c>
+      <c r="D1986">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1987" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1987">
+        <v>199.49999999999901</v>
+      </c>
+      <c r="B1987">
+        <v>0</v>
+      </c>
+      <c r="C1987">
+        <v>0</v>
+      </c>
+      <c r="D1987">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1988" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1988">
+        <v>199.599999999999</v>
+      </c>
+      <c r="B1988">
+        <v>0</v>
+      </c>
+      <c r="C1988">
+        <v>0</v>
+      </c>
+      <c r="D1988">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1989" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1989">
+        <v>199.69999999999899</v>
+      </c>
+      <c r="B1989">
+        <v>0</v>
+      </c>
+      <c r="C1989">
+        <v>0</v>
+      </c>
+      <c r="D1989">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1990" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1990">
+        <v>199.79999999999899</v>
+      </c>
+      <c r="B1990">
+        <v>0</v>
+      </c>
+      <c r="C1990">
+        <v>0</v>
+      </c>
+      <c r="D1990">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1991" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1991">
+        <v>199.89999999999901</v>
+      </c>
+      <c r="B1991">
+        <v>0</v>
+      </c>
+      <c r="C1991">
+        <v>0</v>
+      </c>
+      <c r="D1991">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1992" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1992">
+        <v>199.99999999999901</v>
+      </c>
+      <c r="B1992">
+        <v>0</v>
+      </c>
+      <c r="C1992">
+        <v>0</v>
+      </c>
+      <c r="D1992">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1993" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1993">
+        <v>200.099999999999</v>
+      </c>
+      <c r="B1993">
+        <v>0</v>
+      </c>
+      <c r="C1993">
+        <v>0</v>
+      </c>
+      <c r="D1993">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1994" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1994">
+        <v>200.19999999999899</v>
+      </c>
+      <c r="B1994">
+        <v>0</v>
+      </c>
+      <c r="C1994">
+        <v>0</v>
+      </c>
+      <c r="D1994">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1995" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1995">
+        <v>200.29999999999899</v>
+      </c>
+      <c r="B1995">
+        <v>0</v>
+      </c>
+      <c r="C1995">
+        <v>0</v>
+      </c>
+      <c r="D1995">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1996" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1996">
+        <v>200.39999999999901</v>
+      </c>
+      <c r="B1996">
+        <v>0</v>
+      </c>
+      <c r="C1996">
+        <v>0</v>
+      </c>
+      <c r="D1996">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1997" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1997">
+        <v>200.49999999999901</v>
+      </c>
+      <c r="B1997">
+        <v>0</v>
+      </c>
+      <c r="C1997">
+        <v>0</v>
+      </c>
+      <c r="D1997">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1998" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1998">
+        <v>200.599999999999</v>
+      </c>
+      <c r="B1998">
+        <v>0</v>
+      </c>
+      <c r="C1998">
+        <v>0</v>
+      </c>
+      <c r="D1998">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1999" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1999">
+        <v>200.69999999999899</v>
+      </c>
+      <c r="B1999">
+        <v>0</v>
+      </c>
+      <c r="C1999">
+        <v>0</v>
+      </c>
+      <c r="D1999">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2000" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2000">
+        <v>200.79999999999899</v>
+      </c>
+      <c r="B2000">
+        <v>0</v>
+      </c>
+      <c r="C2000">
+        <v>0</v>
+      </c>
+      <c r="D2000">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2001" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2001">
+        <v>200.89999999999901</v>
+      </c>
+      <c r="B2001">
+        <v>0</v>
+      </c>
+      <c r="C2001">
+        <v>0</v>
+      </c>
+      <c r="D2001">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2002" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2002">
+        <v>200.99999999999901</v>
+      </c>
+      <c r="B2002">
+        <v>0</v>
+      </c>
+      <c r="C2002">
+        <v>0</v>
+      </c>
+      <c r="D2002">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2003" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2003">
+        <v>201.099999999999</v>
+      </c>
+      <c r="B2003">
+        <v>0</v>
+      </c>
+      <c r="C2003">
+        <v>0</v>
+      </c>
+      <c r="D2003">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2004" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2004">
+        <v>201.19999999999899</v>
+      </c>
+      <c r="B2004">
+        <v>0</v>
+      </c>
+      <c r="C2004">
+        <v>0</v>
+      </c>
+      <c r="D2004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2005" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2005">
+        <v>201.29999999999899</v>
+      </c>
+      <c r="B2005">
+        <v>0</v>
+      </c>
+      <c r="C2005">
+        <v>0</v>
+      </c>
+      <c r="D2005">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2006" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2006">
+        <v>201.39999999999901</v>
+      </c>
+      <c r="B2006">
+        <v>0</v>
+      </c>
+      <c r="C2006">
+        <v>0</v>
+      </c>
+      <c r="D2006">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2007" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2007">
+        <v>201.49999999999901</v>
+      </c>
+      <c r="B2007">
+        <v>0</v>
+      </c>
+      <c r="C2007">
+        <v>0</v>
+      </c>
+      <c r="D2007">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2008" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2008">
+        <v>201.599999999999</v>
+      </c>
+      <c r="B2008">
+        <v>0</v>
+      </c>
+      <c r="C2008">
+        <v>0</v>
+      </c>
+      <c r="D2008">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2009" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2009">
+        <v>201.69999999999899</v>
+      </c>
+      <c r="B2009">
+        <v>0</v>
+      </c>
+      <c r="C2009">
+        <v>0</v>
+      </c>
+      <c r="D2009">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2010" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2010">
+        <v>201.79999999999899</v>
+      </c>
+      <c r="B2010">
+        <v>0</v>
+      </c>
+      <c r="C2010">
+        <v>0</v>
+      </c>
+      <c r="D2010">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2011" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2011">
+        <v>201.89999999999901</v>
+      </c>
+      <c r="B2011">
+        <v>0</v>
+      </c>
+      <c r="C2011">
+        <v>0</v>
+      </c>
+      <c r="D2011">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2012" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2012">
+        <v>201.99999999999901</v>
+      </c>
+      <c r="B2012">
+        <v>0</v>
+      </c>
+      <c r="C2012">
+        <v>0</v>
+      </c>
+      <c r="D2012">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2013" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2013">
+        <v>202.099999999999</v>
+      </c>
+      <c r="B2013">
+        <v>0</v>
+      </c>
+      <c r="C2013">
+        <v>0</v>
+      </c>
+      <c r="D2013">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2014" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2014">
+        <v>202.19999999999899</v>
+      </c>
+      <c r="B2014">
+        <v>0</v>
+      </c>
+      <c r="C2014">
+        <v>0</v>
+      </c>
+      <c r="D2014">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2015" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2015">
+        <v>202.29999999999899</v>
+      </c>
+      <c r="B2015">
+        <v>0</v>
+      </c>
+      <c r="C2015">
+        <v>0</v>
+      </c>
+      <c r="D2015">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2016" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2016">
+        <v>202.39999999999901</v>
+      </c>
+      <c r="B2016">
+        <v>0</v>
+      </c>
+      <c r="C2016">
+        <v>0</v>
+      </c>
+      <c r="D2016">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2017" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2017">
+        <v>202.49999999999901</v>
+      </c>
+      <c r="B2017">
+        <v>0</v>
+      </c>
+      <c r="C2017">
+        <v>0</v>
+      </c>
+      <c r="D2017">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2018" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2018">
+        <v>202.599999999999</v>
+      </c>
+      <c r="B2018">
+        <v>0</v>
+      </c>
+      <c r="C2018">
+        <v>0</v>
+      </c>
+      <c r="D2018">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2019" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2019">
+        <v>202.69999999999899</v>
+      </c>
+      <c r="B2019">
+        <v>0</v>
+      </c>
+      <c r="C2019">
+        <v>0</v>
+      </c>
+      <c r="D2019">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2020" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2020">
+        <v>202.79999999999899</v>
+      </c>
+      <c r="B2020">
+        <v>0</v>
+      </c>
+      <c r="C2020">
+        <v>0</v>
+      </c>
+      <c r="D2020">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2021" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2021">
+        <v>202.89999999999901</v>
+      </c>
+      <c r="B2021">
+        <v>0</v>
+      </c>
+      <c r="C2021">
+        <v>0</v>
+      </c>
+      <c r="D2021">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2022" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2022">
+        <v>202.99999999999901</v>
+      </c>
+      <c r="B2022">
+        <v>0</v>
+      </c>
+      <c r="C2022">
+        <v>0</v>
+      </c>
+      <c r="D2022">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2023" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2023">
+        <v>203.099999999999</v>
+      </c>
+      <c r="B2023">
+        <v>0</v>
+      </c>
+      <c r="C2023">
+        <v>0</v>
+      </c>
+      <c r="D2023">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2024" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2024">
+        <v>203.19999999999899</v>
+      </c>
+      <c r="B2024">
+        <v>0</v>
+      </c>
+      <c r="C2024">
+        <v>0</v>
+      </c>
+      <c r="D2024">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2025" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2025">
+        <v>203.29999999999899</v>
+      </c>
+      <c r="B2025">
+        <v>0</v>
+      </c>
+      <c r="C2025">
+        <v>0</v>
+      </c>
+      <c r="D2025">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2026" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2026">
+        <v>203.39999999999901</v>
+      </c>
+      <c r="B2026">
+        <v>0</v>
+      </c>
+      <c r="C2026">
+        <v>0</v>
+      </c>
+      <c r="D2026">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2027" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2027">
+        <v>203.49999999999901</v>
+      </c>
+      <c r="B2027">
+        <v>0</v>
+      </c>
+      <c r="C2027">
+        <v>0</v>
+      </c>
+      <c r="D2027">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2028" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2028">
+        <v>203.599999999999</v>
+      </c>
+      <c r="B2028">
+        <v>0</v>
+      </c>
+      <c r="C2028">
+        <v>0</v>
+      </c>
+      <c r="D2028">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2029" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2029">
+        <v>203.69999999999899</v>
+      </c>
+      <c r="B2029">
+        <v>0</v>
+      </c>
+      <c r="C2029">
+        <v>0</v>
+      </c>
+      <c r="D2029">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2030" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2030">
+        <v>203.79999999999899</v>
+      </c>
+      <c r="B2030">
+        <v>0</v>
+      </c>
+      <c r="C2030">
+        <v>0</v>
+      </c>
+      <c r="D2030">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2031" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2031">
+        <v>203.89999999999901</v>
+      </c>
+      <c r="B2031">
+        <v>0</v>
+      </c>
+      <c r="C2031">
+        <v>0</v>
+      </c>
+      <c r="D2031">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2032" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2032">
+        <v>203.99999999999901</v>
+      </c>
+      <c r="B2032">
+        <v>0</v>
+      </c>
+      <c r="C2032">
+        <v>0</v>
+      </c>
+      <c r="D2032">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2033" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2033">
+        <v>204.099999999999</v>
+      </c>
+      <c r="B2033">
+        <v>0</v>
+      </c>
+      <c r="C2033">
+        <v>0</v>
+      </c>
+      <c r="D2033">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2034" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2034">
+        <v>204.19999999999899</v>
+      </c>
+      <c r="B2034">
+        <v>0</v>
+      </c>
+      <c r="C2034">
+        <v>0</v>
+      </c>
+      <c r="D2034">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2035" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2035">
+        <v>204.29999999999899</v>
+      </c>
+      <c r="B2035">
+        <v>0</v>
+      </c>
+      <c r="C2035">
+        <v>0</v>
+      </c>
+      <c r="D2035">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2036" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2036">
+        <v>204.39999999999901</v>
+      </c>
+      <c r="B2036">
+        <v>0</v>
+      </c>
+      <c r="C2036">
+        <v>0</v>
+      </c>
+      <c r="D2036">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2037" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2037">
+        <v>204.49999999999901</v>
+      </c>
+      <c r="B2037">
+        <v>0</v>
+      </c>
+      <c r="C2037">
+        <v>0</v>
+      </c>
+      <c r="D2037">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2038" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2038">
+        <v>204.599999999999</v>
+      </c>
+      <c r="B2038">
+        <v>0</v>
+      </c>
+      <c r="C2038">
+        <v>0</v>
+      </c>
+      <c r="D2038">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2039" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2039">
+        <v>204.69999999999899</v>
+      </c>
+      <c r="B2039">
+        <v>0</v>
+      </c>
+      <c r="C2039">
+        <v>0</v>
+      </c>
+      <c r="D2039">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2040" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2040">
+        <v>204.79999999999899</v>
+      </c>
+      <c r="B2040">
+        <v>0</v>
+      </c>
+      <c r="C2040">
+        <v>0</v>
+      </c>
+      <c r="D2040">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2041" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2041">
+        <v>204.89999999999901</v>
+      </c>
+      <c r="B2041">
+        <v>0</v>
+      </c>
+      <c r="C2041">
+        <v>0</v>
+      </c>
+      <c r="D2041">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2042" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2042">
+        <v>204.99999999999901</v>
+      </c>
+      <c r="B2042">
+        <v>0</v>
+      </c>
+      <c r="C2042">
+        <v>0</v>
+      </c>
+      <c r="D2042">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2043" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2043">
+        <v>205.099999999999</v>
+      </c>
+      <c r="B2043">
+        <v>0</v>
+      </c>
+      <c r="C2043">
+        <v>0</v>
+      </c>
+      <c r="D2043">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2044" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2044">
+        <v>205.19999999999899</v>
+      </c>
+      <c r="B2044">
+        <v>0</v>
+      </c>
+      <c r="C2044">
+        <v>0</v>
+      </c>
+      <c r="D2044">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2045" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2045">
+        <v>205.29999999999899</v>
+      </c>
+      <c r="B2045">
+        <v>0</v>
+      </c>
+      <c r="C2045">
+        <v>0</v>
+      </c>
+      <c r="D2045">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2046" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2046">
+        <v>205.39999999999901</v>
+      </c>
+      <c r="B2046">
+        <v>0</v>
+      </c>
+      <c r="C2046">
+        <v>0</v>
+      </c>
+      <c r="D2046">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2047" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2047">
+        <v>205.49999999999901</v>
+      </c>
+      <c r="B2047">
+        <v>0</v>
+      </c>
+      <c r="C2047">
+        <v>0</v>
+      </c>
+      <c r="D2047">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2048" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2048">
+        <v>205.599999999999</v>
+      </c>
+      <c r="B2048">
+        <v>0</v>
+      </c>
+      <c r="C2048">
+        <v>0</v>
+      </c>
+      <c r="D2048">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2049" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2049">
+        <v>205.69999999999899</v>
+      </c>
+      <c r="B2049">
+        <v>0</v>
+      </c>
+      <c r="C2049">
+        <v>0</v>
+      </c>
+      <c r="D2049">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2050" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2050">
+        <v>205.79999999999899</v>
+      </c>
+      <c r="B2050">
+        <v>0</v>
+      </c>
+      <c r="C2050">
+        <v>0</v>
+      </c>
+      <c r="D2050">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2051" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2051">
+        <v>205.89999999999901</v>
+      </c>
+      <c r="B2051">
+        <v>0</v>
+      </c>
+      <c r="C2051">
+        <v>0</v>
+      </c>
+      <c r="D2051">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2052" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2052">
+        <v>205.99999999999901</v>
+      </c>
+      <c r="B2052">
+        <v>0</v>
+      </c>
+      <c r="C2052">
+        <v>0</v>
+      </c>
+      <c r="D2052">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2053" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2053">
+        <v>206.099999999999</v>
+      </c>
+      <c r="B2053">
+        <v>0</v>
+      </c>
+      <c r="C2053">
+        <v>0</v>
+      </c>
+      <c r="D2053">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2054" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2054">
+        <v>206.19999999999899</v>
+      </c>
+      <c r="B2054">
+        <v>0</v>
+      </c>
+      <c r="C2054">
+        <v>0</v>
+      </c>
+      <c r="D2054">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2055" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2055">
+        <v>206.29999999999899</v>
+      </c>
+      <c r="B2055">
+        <v>0</v>
+      </c>
+      <c r="C2055">
+        <v>0</v>
+      </c>
+      <c r="D2055">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2056" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2056">
+        <v>206.39999999999901</v>
+      </c>
+      <c r="B2056">
+        <v>0</v>
+      </c>
+      <c r="C2056">
+        <v>0</v>
+      </c>
+      <c r="D2056">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2057" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2057">
+        <v>206.49999999999901</v>
+      </c>
+      <c r="B2057">
+        <v>0</v>
+      </c>
+      <c r="C2057">
+        <v>0</v>
+      </c>
+      <c r="D2057">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2058" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2058">
+        <v>206.599999999999</v>
+      </c>
+      <c r="B2058">
+        <v>0</v>
+      </c>
+      <c r="C2058">
+        <v>0</v>
+      </c>
+      <c r="D2058">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2059" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2059">
+        <v>206.69999999999899</v>
+      </c>
+      <c r="B2059">
+        <v>0</v>
+      </c>
+      <c r="C2059">
+        <v>0</v>
+      </c>
+      <c r="D2059">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2060" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2060">
+        <v>206.79999999999899</v>
+      </c>
+      <c r="B2060">
+        <v>0</v>
+      </c>
+      <c r="C2060">
+        <v>0</v>
+      </c>
+      <c r="D2060">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2061" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2061">
+        <v>206.89999999999901</v>
+      </c>
+      <c r="B2061">
+        <v>0</v>
+      </c>
+      <c r="C2061">
+        <v>0</v>
+      </c>
+      <c r="D2061">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2062" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2062">
+        <v>206.99999999999901</v>
+      </c>
+      <c r="B2062">
+        <v>0</v>
+      </c>
+      <c r="C2062">
+        <v>0</v>
+      </c>
+      <c r="D2062">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2063" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2063">
+        <v>207.099999999999</v>
+      </c>
+      <c r="B2063">
+        <v>0</v>
+      </c>
+      <c r="C2063">
+        <v>0</v>
+      </c>
+      <c r="D2063">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2064" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2064">
+        <v>207.19999999999899</v>
+      </c>
+      <c r="B2064">
+        <v>0</v>
+      </c>
+      <c r="C2064">
+        <v>0</v>
+      </c>
+      <c r="D2064">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2065" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2065">
+        <v>207.29999999999899</v>
+      </c>
+      <c r="B2065">
+        <v>0</v>
+      </c>
+      <c r="C2065">
+        <v>0</v>
+      </c>
+      <c r="D2065">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2066" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2066">
+        <v>207.39999999999901</v>
+      </c>
+      <c r="B2066">
+        <v>0</v>
+      </c>
+      <c r="C2066">
+        <v>0</v>
+      </c>
+      <c r="D2066">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2067" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2067">
+        <v>207.49999999999901</v>
+      </c>
+      <c r="B2067">
+        <v>0</v>
+      </c>
+      <c r="C2067">
+        <v>0</v>
+      </c>
+      <c r="D2067">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2068" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2068">
+        <v>207.599999999999</v>
+      </c>
+      <c r="B2068">
+        <v>0</v>
+      </c>
+      <c r="C2068">
+        <v>0</v>
+      </c>
+      <c r="D2068">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2069" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2069">
+        <v>207.69999999999899</v>
+      </c>
+      <c r="B2069">
+        <v>0</v>
+      </c>
+      <c r="C2069">
+        <v>0</v>
+      </c>
+      <c r="D2069">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2070" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2070">
+        <v>207.79999999999899</v>
+      </c>
+      <c r="B2070">
+        <v>0</v>
+      </c>
+      <c r="C2070">
+        <v>0</v>
+      </c>
+      <c r="D2070">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2071" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2071">
+        <v>207.89999999999901</v>
+      </c>
+      <c r="B2071">
+        <v>0</v>
+      </c>
+      <c r="C2071">
+        <v>0</v>
+      </c>
+      <c r="D2071">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2072" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2072">
+        <v>207.99999999999901</v>
+      </c>
+      <c r="B2072">
+        <v>0</v>
+      </c>
+      <c r="C2072">
+        <v>0</v>
+      </c>
+      <c r="D2072">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2073" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2073">
+        <v>208.099999999999</v>
+      </c>
+      <c r="B2073">
+        <v>0</v>
+      </c>
+      <c r="C2073">
+        <v>0</v>
+      </c>
+      <c r="D2073">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2074" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2074">
+        <v>208.19999999999899</v>
+      </c>
+      <c r="B2074">
+        <v>0</v>
+      </c>
+      <c r="C2074">
+        <v>0</v>
+      </c>
+      <c r="D2074">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2075" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2075">
+        <v>208.29999999999899</v>
+      </c>
+      <c r="B2075">
+        <v>0</v>
+      </c>
+      <c r="C2075">
+        <v>0</v>
+      </c>
+      <c r="D2075">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2076" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2076">
+        <v>208.39999999999901</v>
+      </c>
+      <c r="B2076">
+        <v>0</v>
+      </c>
+      <c r="C2076">
+        <v>0</v>
+      </c>
+      <c r="D2076">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2077" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2077">
+        <v>208.49999999999901</v>
+      </c>
+      <c r="B2077">
+        <v>0</v>
+      </c>
+      <c r="C2077">
+        <v>0</v>
+      </c>
+      <c r="D2077">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2078" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2078">
+        <v>208.599999999999</v>
+      </c>
+      <c r="B2078">
+        <v>0</v>
+      </c>
+      <c r="C2078">
+        <v>0</v>
+      </c>
+      <c r="D2078">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2079" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2079">
+        <v>208.69999999999899</v>
+      </c>
+      <c r="B2079">
+        <v>0</v>
+      </c>
+      <c r="C2079">
+        <v>0</v>
+      </c>
+      <c r="D2079">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2080" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2080">
+        <v>208.79999999999899</v>
+      </c>
+      <c r="B2080">
+        <v>0</v>
+      </c>
+      <c r="C2080">
+        <v>0</v>
+      </c>
+      <c r="D2080">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2081" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2081">
+        <v>208.89999999999901</v>
+      </c>
+      <c r="B2081">
+        <v>0</v>
+      </c>
+      <c r="C2081">
+        <v>0</v>
+      </c>
+      <c r="D2081">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2082" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2082">
+        <v>208.99999999999901</v>
+      </c>
+      <c r="B2082">
+        <v>0</v>
+      </c>
+      <c r="C2082">
+        <v>0</v>
+      </c>
+      <c r="D2082">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2083" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2083">
+        <v>209.099999999999</v>
+      </c>
+      <c r="B2083">
+        <v>0</v>
+      </c>
+      <c r="C2083">
+        <v>0</v>
+      </c>
+      <c r="D2083">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2084" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2084">
+        <v>209.19999999999899</v>
+      </c>
+      <c r="B2084">
+        <v>0</v>
+      </c>
+      <c r="C2084">
+        <v>0</v>
+      </c>
+      <c r="D2084">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2085" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2085">
+        <v>209.29999999999899</v>
+      </c>
+      <c r="B2085">
+        <v>0</v>
+      </c>
+      <c r="C2085">
+        <v>0</v>
+      </c>
+      <c r="D2085">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2086" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2086">
+        <v>209.39999999999901</v>
+      </c>
+      <c r="B2086">
+        <v>0</v>
+      </c>
+      <c r="C2086">
+        <v>0</v>
+      </c>
+      <c r="D2086">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2087" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2087">
+        <v>209.49999999999901</v>
+      </c>
+      <c r="B2087">
+        <v>0</v>
+      </c>
+      <c r="C2087">
+        <v>0</v>
+      </c>
+      <c r="D2087">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2088" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2088">
+        <v>209.599999999999</v>
+      </c>
+      <c r="B2088">
+        <v>0</v>
+      </c>
+      <c r="C2088">
+        <v>0</v>
+      </c>
+      <c r="D2088">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2089" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2089">
+        <v>209.69999999999899</v>
+      </c>
+      <c r="B2089">
+        <v>0</v>
+      </c>
+      <c r="C2089">
+        <v>0</v>
+      </c>
+      <c r="D2089">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2090" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2090">
+        <v>209.79999999999899</v>
+      </c>
+      <c r="B2090">
+        <v>0</v>
+      </c>
+      <c r="C2090">
+        <v>0</v>
+      </c>
+      <c r="D2090">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2091" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2091">
+        <v>209.89999999999901</v>
+      </c>
+      <c r="B2091">
+        <v>0</v>
+      </c>
+      <c r="C2091">
+        <v>0</v>
+      </c>
+      <c r="D2091">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2092" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2092">
+        <v>209.99999999999901</v>
+      </c>
+      <c r="B2092">
+        <v>0</v>
+      </c>
+      <c r="C2092">
+        <v>0</v>
+      </c>
+      <c r="D2092">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>